<commit_message>
update 3ds case for brick 1.6
</commit_message>
<xml_diff>
--- a/src/main/java/utility/cardNumber_v1.xlsx
+++ b/src/main/java/utility/cardNumber_v1.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC53FB7F-5D3A-4F82-88B7-EA0A956562C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F0D336-260B-40C8-9BF5-8A55A575113E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -19,6 +18,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="141">
   <si>
     <t>caseID</t>
   </si>
@@ -591,117 +591,6 @@
   </si>
   <si>
     <t>5200 0000 0000 0007</t>
-  </si>
-  <si>
-    <t>STATUS_AWAITING_PAYMENT</t>
-  </si>
-  <si>
-    <t>STATUS_IN_REVIEW</t>
-  </si>
-  <si>
-    <t>STATUS_PAY</t>
-  </si>
-  <si>
-    <t>STATUS_AVAILABLE</t>
-  </si>
-  <si>
-    <t>STATUS_IN_DISPUTE</t>
-  </si>
-  <si>
-    <t>STATUS_RETURNED</t>
-  </si>
-  <si>
-    <t>STATUS_CANCELED</t>
-  </si>
-  <si>
-    <t>STATUS_DEBITED</t>
-  </si>
-  <si>
-    <t>STATUS_CHARGEBACK</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Canceled</t>
-  </si>
-  <si>
-    <t>Chargeback</t>
-  </si>
-  <si>
-    <t>Refunded</t>
-  </si>
-  <si>
-    <t>Devolvida</t>
-  </si>
-  <si>
-    <t>Disponível</t>
-  </si>
-  <si>
-    <t>Paga</t>
-  </si>
-  <si>
-    <t>Paid</t>
-  </si>
-  <si>
-    <t>Chargeback debitado</t>
-  </si>
-  <si>
-    <t>Contested</t>
-  </si>
-  <si>
-    <t>Cancelada</t>
-  </si>
-  <si>
-    <t>Em disputa</t>
-  </si>
-  <si>
-    <t>Em contestação</t>
-  </si>
-  <si>
-    <t>Em devolução</t>
-  </si>
-  <si>
-    <t>In dispute</t>
-  </si>
-  <si>
-    <t>Em análise</t>
-  </si>
-  <si>
-    <t>In review</t>
-  </si>
-  <si>
-    <t>Aguardando pagamento</t>
-  </si>
-  <si>
-    <t>Awaiting Payment</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Meaning</t>
-  </si>
-  <si>
-    <t>Portugese</t>
-  </si>
-  <si>
-    <t>PW</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -1132,9 +1021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,206 +2877,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" t="s">
-        <v>159</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>